<commit_message>
Update helper xlsx - removed rounding up to next hour
</commit_message>
<xml_diff>
--- a/resources/ResStock-CalcNumberSims.xlsx
+++ b/resources/ResStock-CalcNumberSims.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-51200" yWindow="-10340" windowWidth="51200" windowHeight="28340" tabRatio="500"/>
+    <workbookView xWindow="-51200" yWindow="-10340" windowWidth="51200" windowHeight="28240" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Calc" sheetId="3" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="263">
   <si>
     <t>Option=CR02</t>
   </si>
@@ -816,6 +816,12 @@
   </si>
   <si>
     <t>Location(s) - See map at right for coverage</t>
+  </si>
+  <si>
+    <t>Forgetfulness penalty (hr)</t>
+  </si>
+  <si>
+    <t>Minimum Possible Cost</t>
   </si>
 </sst>
 </file>
@@ -1076,20 +1082,30 @@
   <c:chart>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.102971503373037"/>
+          <c:y val="0.0470730190627194"/>
+          <c:w val="0.50162667741471"/>
+          <c:h val="0.776378924402898"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
+          <c:idx val="2"/>
+          <c:order val="0"/>
           <c:tx>
             <c:strRef>
               <c:f>Calc!$W$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Cost</c:v>
+                  <c:v>Minimum Possible Cost</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1263,154 +1279,499 @@
                 <c:formatCode>"$"#,##0.00;[Red]"$"#,##0.00</c:formatCode>
                 <c:ptCount val="50"/>
                 <c:pt idx="0">
-                  <c:v>31.08</c:v>
+                  <c:v>30.53801574859587</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>30.6</c:v>
+                  <c:v>26.78641676228188</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>31.2</c:v>
+                  <c:v>25.03567056866869</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>28.44</c:v>
+                  <c:v>24.02208066710315</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>33.48</c:v>
+                  <c:v>23.36104377477781</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>25.68</c:v>
+                  <c:v>22.89586966536367</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>29.04</c:v>
+                  <c:v>22.55074048741125</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>32.4</c:v>
+                  <c:v>22.28449797870509</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>35.76</c:v>
+                  <c:v>22.07286931793866</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>39.12</c:v>
+                  <c:v>21.90061343126832</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>42.48</c:v>
+                  <c:v>21.75767769552058</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>22.92</c:v>
+                  <c:v>21.63716325165484</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>24.6</c:v>
+                  <c:v>21.5341781814423</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>26.28</c:v>
+                  <c:v>21.44515718854671</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>27.96</c:v>
+                  <c:v>21.36744044871723</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>29.64</c:v>
+                  <c:v>21.29900331961366</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>31.32</c:v>
+                  <c:v>21.23827741632457</c:v>
                 </c:pt>
                 <c:pt idx="17">
+                  <c:v>21.18402894271966</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>21.13527398542917</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>21.09121830113052</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21.05121371423866</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>21.01472601410652</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>20.98131096240655</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>20.95059611690456</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>20.9222668904707</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>20.89605573704123</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>20.87173367575082</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>20.84910358394148</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>20.82799484284202</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>20.80825902799292</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>20.78976641407921</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>20.77240312009916</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>20.75606876205865</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>20.74067451095574</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>20.72614147669774</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>20.71239935586876</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>20.69938529442144</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>20.68704292646817</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>20.67532155816036</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>20.66417547173267</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>20.653563329565</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>20.64344766188471</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>20.63379442472694</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>20.62457261716282</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>20.61575394872718</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>20.60731254952943</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>20.59922471679022</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>20.59146869257365</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>20.58402446832559</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>20.5768736125208</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Calc!$X$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Cost w/ 1 hr of extra time that clusters are running</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:prstDash val="sysDash"/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Calc!$U$4:$U$53</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>22.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>24.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>26.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>27.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>28.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>29.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>31.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
                   <c:v>33.0</c:v>
                 </c:pt>
+                <c:pt idx="33">
+                  <c:v>34.0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>35.0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>36.0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>37.0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>38.0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>39.0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>41.0</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>43.0</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>44.0</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>45.0</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>46.0</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>48.0</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>49.0</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>50.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Calc!$X$4:$X$53</c:f>
+              <c:numCache>
+                <c:formatCode>"$"#,##0.00;[Red]"$"#,##0.00</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>34.97801574859587</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32.90641676228188</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32.83567056866868</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>33.50208066710316</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>34.52104377477781</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>35.73586966536367</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>37.07074048741126</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>38.48449797870509</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>39.95286931793866</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>41.46061343126831</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>42.99767769552059</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>44.55716325165483</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>46.13417818144229</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>47.7251571885467</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>49.32744044871723</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>50.93900331961366</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>52.55827741632457</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>54.18402894271965</c:v>
+                </c:pt>
                 <c:pt idx="18">
-                  <c:v>34.68</c:v>
+                  <c:v>55.81527398542917</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>36.36</c:v>
+                  <c:v>57.45121830113052</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>38.04</c:v>
+                  <c:v>59.09121371423866</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>39.72</c:v>
+                  <c:v>60.73472601410651</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>41.4</c:v>
+                  <c:v>62.38131096240654</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>43.08</c:v>
+                  <c:v>64.03059611690458</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>44.76</c:v>
+                  <c:v>65.6822668904707</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>46.44</c:v>
+                  <c:v>67.33605573704122</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>48.12</c:v>
+                  <c:v>68.99173367575082</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>49.8</c:v>
+                  <c:v>70.64910358394148</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>51.48</c:v>
+                  <c:v>72.307994842842</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>53.16</c:v>
+                  <c:v>73.9682590279929</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>54.84</c:v>
+                  <c:v>75.62976641407921</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>56.52</c:v>
+                  <c:v>77.29240312009915</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>58.2</c:v>
+                  <c:v>78.95606876205865</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>59.88</c:v>
+                  <c:v>80.62067451095574</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>61.56</c:v>
+                  <c:v>82.28614147669774</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>63.24</c:v>
+                  <c:v>83.95239935586876</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>64.92</c:v>
+                  <c:v>85.61938529442145</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>66.6</c:v>
+                  <c:v>87.28704292646817</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>68.28</c:v>
+                  <c:v>88.95532155816034</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>69.96</c:v>
+                  <c:v>90.62417547173267</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>71.64</c:v>
+                  <c:v>92.293563329565</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>73.32000000000001</c:v>
+                  <c:v>93.9634476618847</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>75.0</c:v>
+                  <c:v>95.63379442472694</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>76.68000000000001</c:v>
+                  <c:v>97.30457261716282</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>78.36</c:v>
+                  <c:v>98.97575394872718</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>80.04</c:v>
+                  <c:v>100.6473125495294</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>81.72</c:v>
+                  <c:v>102.3192247167902</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>83.4</c:v>
+                  <c:v>103.9914686925736</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>85.08</c:v>
+                  <c:v>105.6640244683256</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>86.76</c:v>
+                  <c:v>107.3368736125208</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1425,15 +1786,15 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-561514544"/>
-        <c:axId val="-561513664"/>
+        <c:axId val="-578259216"/>
+        <c:axId val="-578257024"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
-          <c:order val="0"/>
+          <c:order val="1"/>
           <c:tx>
             <c:strRef>
               <c:f>Calc!$V$3</c:f>
@@ -1776,17 +2137,27 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-561507760"/>
-        <c:axId val="-561510608"/>
+        <c:axId val="-578240592"/>
+        <c:axId val="-578277536"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-561514544"/>
+        <c:axId val="-578259216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorGridlines/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -1810,18 +2181,28 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-561513664"/>
+        <c:crossAx val="-578257024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-561513664"/>
+        <c:axId val="-578257024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -1850,12 +2231,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-561514544"/>
+        <c:crossAx val="-578259216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-561510608"/>
+        <c:axId val="-578277536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1884,12 +2265,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-561507760"/>
+        <c:crossAx val="-578240592"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-561507760"/>
+        <c:axId val="-578240592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1899,14 +2280,23 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-561510608"/>
+        <c:crossAx val="-578277536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.7034044220859"/>
+          <c:y val="0.325291098580482"/>
+          <c:w val="0.284544358333051"/>
+          <c:h val="0.34941751772081"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2783,15 +3173,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>110067</xdr:colOff>
+      <xdr:colOff>88901</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>122767</xdr:rowOff>
+      <xdr:rowOff>133351</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>465667</xdr:colOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>264583</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>10584</xdr:rowOff>
+      <xdr:rowOff>21168</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2819,7 +3209,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>765190</xdr:colOff>
+      <xdr:colOff>468856</xdr:colOff>
       <xdr:row>55</xdr:row>
       <xdr:rowOff>148166</xdr:rowOff>
     </xdr:to>
@@ -3210,10 +3600,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:W65"/>
+  <dimension ref="B2:X65"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="Y6" sqref="Y6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3222,16 +3612,16 @@
     <col min="2" max="2" width="72.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="10.83203125" style="1"/>
-    <col min="6" max="6" width="18" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B2" s="4" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="3" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B3" s="4" t="s">
         <v>246</v>
       </c>
@@ -3242,10 +3632,14 @@
         <v>254</v>
       </c>
       <c r="W3" s="10" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="4" spans="2:23" x14ac:dyDescent="0.2">
+        <v>262</v>
+      </c>
+      <c r="X3" s="10" t="str">
+        <f>"Cost w/ "&amp;G10&amp;" hr of extra time that clusters are running"</f>
+        <v>Cost w/ 1 hr of extra time that clusters are running</v>
+      </c>
+    </row>
+    <row r="4" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
         <v>244</v>
       </c>
@@ -3267,11 +3661,15 @@
         <v>6.8779314749089808</v>
       </c>
       <c r="W4" s="12">
-        <f>(CEILING(V4,1))*U4*$G$8+(CEILING(V4,1))*$G$9</f>
-        <v>31.08</v>
-      </c>
-    </row>
-    <row r="5" spans="2:23" x14ac:dyDescent="0.2">
+        <f>(V4)*U4*$G$8+(V4)*$G$9</f>
+        <v>30.538015748595875</v>
+      </c>
+      <c r="X4" s="12">
+        <f>(V4+$G$10)*U4*$G$8+(V4+$G$10)*$G$9</f>
+        <v>34.978015748595872</v>
+      </c>
+    </row>
+    <row r="5" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
         <v>243</v>
       </c>
@@ -3293,11 +3691,15 @@
         <v>4.3768654840329875</v>
       </c>
       <c r="W5" s="12">
-        <f t="shared" ref="W5:W54" si="0">(CEILING(V5,1))*U5*$G$8+(CEILING(V5,1))*$G$9</f>
-        <v>30.6</v>
-      </c>
-    </row>
-    <row r="6" spans="2:23" x14ac:dyDescent="0.2">
+        <f t="shared" ref="W5:W54" si="0">(V5)*U5*$G$8+(V5)*$G$9</f>
+        <v>26.786416762281881</v>
+      </c>
+      <c r="X5" s="12">
+        <f t="shared" ref="X5:X54" si="1">(V5+$G$10)*U5*$G$8+(V5+$G$10)*$G$9</f>
+        <v>32.906416762281879</v>
+      </c>
+    </row>
+    <row r="6" spans="2:24" x14ac:dyDescent="0.2">
       <c r="F6" s="1" t="s">
         <v>237</v>
       </c>
@@ -3314,10 +3716,14 @@
       </c>
       <c r="W6" s="12">
         <f t="shared" si="0"/>
-        <v>31.2</v>
-      </c>
-    </row>
-    <row r="7" spans="2:23" ht="32" x14ac:dyDescent="0.2">
+        <v>25.035670568668689</v>
+      </c>
+      <c r="X6" s="12">
+        <f t="shared" si="1"/>
+        <v>32.835670568668682</v>
+      </c>
+    </row>
+    <row r="7" spans="2:24" ht="32" x14ac:dyDescent="0.2">
       <c r="B7" s="13" t="s">
         <v>259</v>
       </c>
@@ -3336,10 +3742,14 @@
       </c>
       <c r="W7" s="12">
         <f t="shared" si="0"/>
-        <v>28.439999999999998</v>
-      </c>
-    </row>
-    <row r="8" spans="2:23" x14ac:dyDescent="0.2">
+        <v>24.022080667103154</v>
+      </c>
+      <c r="X7" s="12">
+        <f t="shared" si="1"/>
+        <v>33.502080667103158</v>
+      </c>
+    </row>
+    <row r="8" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
         <v>247</v>
       </c>
@@ -3362,10 +3772,14 @@
       </c>
       <c r="W8" s="12">
         <f t="shared" si="0"/>
-        <v>33.479999999999997</v>
-      </c>
-    </row>
-    <row r="9" spans="2:23" x14ac:dyDescent="0.2">
+        <v>23.361043774777809</v>
+      </c>
+      <c r="X8" s="12">
+        <f t="shared" si="1"/>
+        <v>34.521043774777809</v>
+      </c>
+    </row>
+    <row r="9" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
         <v>251</v>
       </c>
@@ -3387,10 +3801,14 @@
       </c>
       <c r="W9" s="12">
         <f t="shared" si="0"/>
-        <v>25.68</v>
-      </c>
-    </row>
-    <row r="10" spans="2:23" x14ac:dyDescent="0.2">
+        <v>22.895869665363673</v>
+      </c>
+      <c r="X9" s="12">
+        <f t="shared" si="1"/>
+        <v>35.735869665363673</v>
+      </c>
+    </row>
+    <row r="10" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
         <v>252</v>
       </c>
@@ -3399,7 +3817,7 @@
         <v>4.3768654840329875</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>256</v>
+        <v>261</v>
       </c>
       <c r="G10" s="1">
         <v>1</v>
@@ -3413,16 +3831,20 @@
       </c>
       <c r="W10" s="12">
         <f t="shared" si="0"/>
-        <v>29.04</v>
-      </c>
-    </row>
-    <row r="11" spans="2:23" x14ac:dyDescent="0.2">
+        <v>22.550740487411247</v>
+      </c>
+      <c r="X10" s="12">
+        <f t="shared" si="1"/>
+        <v>37.070740487411257</v>
+      </c>
+    </row>
+    <row r="11" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
         <v>249</v>
       </c>
       <c r="C11" s="9">
-        <f>(CEILING($C$10,1))*$C$9*$G$8+(CEILING($C$10,1))*$G$9</f>
-        <v>30.6</v>
+        <f>(($C$10))*$C$9*$G$8+(($C$10))*$G$9</f>
+        <v>26.786416762281881</v>
       </c>
       <c r="U11" s="10">
         <v>8</v>
@@ -3433,10 +3855,14 @@
       </c>
       <c r="W11" s="12">
         <f t="shared" si="0"/>
-        <v>32.4</v>
-      </c>
-    </row>
-    <row r="12" spans="2:23" x14ac:dyDescent="0.2">
+        <v>22.284497978705094</v>
+      </c>
+      <c r="X11" s="12">
+        <f t="shared" si="1"/>
+        <v>38.484497978705093</v>
+      </c>
+    </row>
+    <row r="12" spans="2:24" x14ac:dyDescent="0.2">
       <c r="U12" s="10">
         <v>9</v>
       </c>
@@ -3446,10 +3872,14 @@
       </c>
       <c r="W12" s="12">
         <f t="shared" si="0"/>
-        <v>35.76</v>
-      </c>
-    </row>
-    <row r="13" spans="2:23" x14ac:dyDescent="0.2">
+        <v>22.072869317938665</v>
+      </c>
+      <c r="X12" s="12">
+        <f t="shared" si="1"/>
+        <v>39.952869317938664</v>
+      </c>
+    </row>
+    <row r="13" spans="2:24" x14ac:dyDescent="0.2">
       <c r="U13" s="10">
         <v>10</v>
       </c>
@@ -3459,10 +3889,14 @@
       </c>
       <c r="W13" s="12">
         <f t="shared" si="0"/>
-        <v>39.120000000000005</v>
-      </c>
-    </row>
-    <row r="14" spans="2:23" x14ac:dyDescent="0.2">
+        <v>21.900613431268315</v>
+      </c>
+      <c r="X13" s="12">
+        <f t="shared" si="1"/>
+        <v>41.460613431268307</v>
+      </c>
+    </row>
+    <row r="14" spans="2:24" x14ac:dyDescent="0.2">
       <c r="U14" s="10">
         <v>11</v>
       </c>
@@ -3472,10 +3906,14 @@
       </c>
       <c r="W14" s="12">
         <f t="shared" si="0"/>
-        <v>42.480000000000004</v>
-      </c>
-    </row>
-    <row r="15" spans="2:23" x14ac:dyDescent="0.2">
+        <v>21.757677695520581</v>
+      </c>
+      <c r="X14" s="12">
+        <f t="shared" si="1"/>
+        <v>42.997677695520586</v>
+      </c>
+    </row>
+    <row r="15" spans="2:24" x14ac:dyDescent="0.2">
       <c r="U15" s="10">
         <v>12</v>
       </c>
@@ -3485,10 +3923,14 @@
       </c>
       <c r="W15" s="12">
         <f t="shared" si="0"/>
-        <v>22.92</v>
-      </c>
-    </row>
-    <row r="16" spans="2:23" x14ac:dyDescent="0.2">
+        <v>21.63716325165484</v>
+      </c>
+      <c r="X15" s="12">
+        <f t="shared" si="1"/>
+        <v>44.557163251654835</v>
+      </c>
+    </row>
+    <row r="16" spans="2:24" x14ac:dyDescent="0.2">
       <c r="U16" s="10">
         <v>13</v>
       </c>
@@ -3498,10 +3940,14 @@
       </c>
       <c r="W16" s="12">
         <f t="shared" si="0"/>
-        <v>24.6</v>
-      </c>
-    </row>
-    <row r="17" spans="2:23" x14ac:dyDescent="0.2">
+        <v>21.534178181442297</v>
+      </c>
+      <c r="X16" s="12">
+        <f t="shared" si="1"/>
+        <v>46.134178181442294</v>
+      </c>
+    </row>
+    <row r="17" spans="2:24" x14ac:dyDescent="0.2">
       <c r="U17" s="10">
         <v>14</v>
       </c>
@@ -3511,10 +3957,14 @@
       </c>
       <c r="W17" s="12">
         <f t="shared" si="0"/>
-        <v>26.28</v>
-      </c>
-    </row>
-    <row r="18" spans="2:23" x14ac:dyDescent="0.2">
+        <v>21.445157188546712</v>
+      </c>
+      <c r="X17" s="12">
+        <f t="shared" si="1"/>
+        <v>47.72515718854671</v>
+      </c>
+    </row>
+    <row r="18" spans="2:24" x14ac:dyDescent="0.2">
       <c r="U18" s="10">
         <v>15</v>
       </c>
@@ -3524,10 +3974,14 @@
       </c>
       <c r="W18" s="12">
         <f t="shared" si="0"/>
-        <v>27.96</v>
-      </c>
-    </row>
-    <row r="19" spans="2:23" x14ac:dyDescent="0.2">
+        <v>21.367440448717232</v>
+      </c>
+      <c r="X18" s="12">
+        <f t="shared" si="1"/>
+        <v>49.327440448717233</v>
+      </c>
+    </row>
+    <row r="19" spans="2:24" x14ac:dyDescent="0.2">
       <c r="U19" s="10">
         <v>16</v>
       </c>
@@ -3537,10 +3991,14 @@
       </c>
       <c r="W19" s="12">
         <f t="shared" si="0"/>
-        <v>29.64</v>
-      </c>
-    </row>
-    <row r="20" spans="2:23" x14ac:dyDescent="0.2">
+        <v>21.299003319613661</v>
+      </c>
+      <c r="X19" s="12">
+        <f t="shared" si="1"/>
+        <v>50.939003319613661</v>
+      </c>
+    </row>
+    <row r="20" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B20" s="4" t="s">
         <v>260</v>
       </c>
@@ -3559,10 +4017,14 @@
       </c>
       <c r="W20" s="12">
         <f t="shared" si="0"/>
-        <v>31.32</v>
-      </c>
-    </row>
-    <row r="21" spans="2:23" x14ac:dyDescent="0.2">
+        <v>21.238277416324575</v>
+      </c>
+      <c r="X20" s="12">
+        <f t="shared" si="1"/>
+        <v>52.558277416324572</v>
+      </c>
+    </row>
+    <row r="21" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B21" s="7" t="s">
         <v>74</v>
       </c>
@@ -3583,10 +4045,14 @@
       </c>
       <c r="W21" s="12">
         <f t="shared" si="0"/>
-        <v>33</v>
-      </c>
-    </row>
-    <row r="22" spans="2:23" x14ac:dyDescent="0.2">
+        <v>21.184028942719657</v>
+      </c>
+      <c r="X21" s="12">
+        <f t="shared" si="1"/>
+        <v>54.18402894271965</v>
+      </c>
+    </row>
+    <row r="22" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B22" s="7" t="s">
         <v>81</v>
       </c>
@@ -3607,10 +4073,14 @@
       </c>
       <c r="W22" s="12">
         <f t="shared" si="0"/>
-        <v>34.68</v>
-      </c>
-    </row>
-    <row r="23" spans="2:23" x14ac:dyDescent="0.2">
+        <v>21.135273985429166</v>
+      </c>
+      <c r="X22" s="12">
+        <f t="shared" si="1"/>
+        <v>55.815273985429165</v>
+      </c>
+    </row>
+    <row r="23" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B23" s="7"/>
       <c r="C23" s="5">
         <f>IFERROR(VLOOKUP(B23,'Location EPW.tsv'!$A$15:$L$230,12,FALSE),0)</f>
@@ -3629,10 +4099,14 @@
       </c>
       <c r="W23" s="12">
         <f t="shared" si="0"/>
-        <v>36.36</v>
-      </c>
-    </row>
-    <row r="24" spans="2:23" x14ac:dyDescent="0.2">
+        <v>21.091218301130525</v>
+      </c>
+      <c r="X23" s="12">
+        <f t="shared" si="1"/>
+        <v>57.451218301130524</v>
+      </c>
+    </row>
+    <row r="24" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B24" s="7"/>
       <c r="C24" s="5">
         <f>IFERROR(VLOOKUP(B24,'Location EPW.tsv'!$A$15:$L$230,12,FALSE),0)</f>
@@ -3651,10 +4125,14 @@
       </c>
       <c r="W24" s="12">
         <f t="shared" si="0"/>
-        <v>38.04</v>
-      </c>
-    </row>
-    <row r="25" spans="2:23" x14ac:dyDescent="0.2">
+        <v>21.051213714238656</v>
+      </c>
+      <c r="X24" s="12">
+        <f t="shared" si="1"/>
+        <v>59.091213714238663</v>
+      </c>
+    </row>
+    <row r="25" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B25" s="7"/>
       <c r="C25" s="5">
         <f>IFERROR(VLOOKUP(B25,'Location EPW.tsv'!$A$15:$L$230,12,FALSE),0)</f>
@@ -3673,17 +4151,21 @@
       </c>
       <c r="W25" s="12">
         <f t="shared" si="0"/>
-        <v>39.72</v>
-      </c>
-    </row>
-    <row r="26" spans="2:23" x14ac:dyDescent="0.2">
+        <v>21.014726014106518</v>
+      </c>
+      <c r="X25" s="12">
+        <f t="shared" si="1"/>
+        <v>60.734726014106514</v>
+      </c>
+    </row>
+    <row r="26" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B26" s="7"/>
       <c r="C26" s="5">
         <f>IFERROR(VLOOKUP(B26,'Location EPW.tsv'!$A$15:$L$230,12,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="D26" s="6">
-        <f t="shared" ref="D26:D65" si="1">C26/$G$6</f>
+        <f t="shared" ref="D26:D65" si="2">C26/$G$6</f>
         <v>0</v>
       </c>
       <c r="U26" s="10">
@@ -3695,17 +4177,21 @@
       </c>
       <c r="W26" s="12">
         <f t="shared" si="0"/>
-        <v>41.4</v>
-      </c>
-    </row>
-    <row r="27" spans="2:23" x14ac:dyDescent="0.2">
+        <v>20.98131096240655</v>
+      </c>
+      <c r="X26" s="12">
+        <f t="shared" si="1"/>
+        <v>62.381310962406545</v>
+      </c>
+    </row>
+    <row r="27" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B27" s="7"/>
       <c r="C27" s="5">
         <f>IFERROR(VLOOKUP(B27,'Location EPW.tsv'!$A$15:$L$230,12,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="D27" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="U27" s="10">
@@ -3717,10 +4203,14 @@
       </c>
       <c r="W27" s="12">
         <f t="shared" si="0"/>
-        <v>43.08</v>
-      </c>
-    </row>
-    <row r="28" spans="2:23" x14ac:dyDescent="0.2">
+        <v>20.950596116904563</v>
+      </c>
+      <c r="X27" s="12">
+        <f t="shared" si="1"/>
+        <v>64.030596116904576</v>
+      </c>
+    </row>
+    <row r="28" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B28" s="7"/>
       <c r="C28" s="5"/>
       <c r="D28" s="6"/>
@@ -3733,17 +4223,21 @@
       </c>
       <c r="W28" s="12">
         <f t="shared" si="0"/>
-        <v>44.76</v>
-      </c>
-    </row>
-    <row r="29" spans="2:23" x14ac:dyDescent="0.2">
+        <v>20.922266890470699</v>
+      </c>
+      <c r="X28" s="12">
+        <f t="shared" si="1"/>
+        <v>65.6822668904707</v>
+      </c>
+    </row>
+    <row r="29" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B29" s="7"/>
       <c r="C29" s="5">
         <f>IFERROR(VLOOKUP(B29,'Location EPW.tsv'!$A$15:$L$230,12,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="D29" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="U29" s="10">
@@ -3755,17 +4249,21 @@
       </c>
       <c r="W29" s="12">
         <f t="shared" si="0"/>
-        <v>46.44</v>
-      </c>
-    </row>
-    <row r="30" spans="2:23" x14ac:dyDescent="0.2">
+        <v>20.89605573704123</v>
+      </c>
+      <c r="X29" s="12">
+        <f t="shared" si="1"/>
+        <v>67.336055737041221</v>
+      </c>
+    </row>
+    <row r="30" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B30" s="7"/>
       <c r="C30" s="5">
         <f>IFERROR(VLOOKUP(B30,'Location EPW.tsv'!$A$15:$L$230,12,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="D30" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="U30" s="10">
@@ -3777,17 +4275,21 @@
       </c>
       <c r="W30" s="12">
         <f t="shared" si="0"/>
-        <v>48.12</v>
-      </c>
-    </row>
-    <row r="31" spans="2:23" x14ac:dyDescent="0.2">
+        <v>20.871733675750818</v>
+      </c>
+      <c r="X30" s="12">
+        <f t="shared" si="1"/>
+        <v>68.991733675750822</v>
+      </c>
+    </row>
+    <row r="31" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B31" s="7"/>
       <c r="C31" s="5">
         <f>IFERROR(VLOOKUP(B31,'Location EPW.tsv'!$A$15:$L$230,12,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="D31" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="U31" s="10">
@@ -3799,17 +4301,21 @@
       </c>
       <c r="W31" s="12">
         <f t="shared" si="0"/>
-        <v>49.8</v>
-      </c>
-    </row>
-    <row r="32" spans="2:23" x14ac:dyDescent="0.2">
+        <v>20.849103583941481</v>
+      </c>
+      <c r="X31" s="12">
+        <f t="shared" si="1"/>
+        <v>70.649103583941482</v>
+      </c>
+    </row>
+    <row r="32" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B32" s="7"/>
       <c r="C32" s="5">
         <f>IFERROR(VLOOKUP(B32,'Location EPW.tsv'!$A$15:$L$230,12,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="D32" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="U32" s="10">
@@ -3821,17 +4327,21 @@
       </c>
       <c r="W32" s="12">
         <f t="shared" si="0"/>
-        <v>51.48</v>
-      </c>
-    </row>
-    <row r="33" spans="2:23" x14ac:dyDescent="0.2">
+        <v>20.827994842842021</v>
+      </c>
+      <c r="X32" s="12">
+        <f t="shared" si="1"/>
+        <v>72.307994842842007</v>
+      </c>
+    </row>
+    <row r="33" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B33" s="7"/>
       <c r="C33" s="5">
         <f>IFERROR(VLOOKUP(B33,'Location EPW.tsv'!$A$15:$L$230,12,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="D33" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="U33" s="10">
@@ -3843,17 +4353,21 @@
       </c>
       <c r="W33" s="12">
         <f t="shared" si="0"/>
-        <v>53.16</v>
-      </c>
-    </row>
-    <row r="34" spans="2:23" x14ac:dyDescent="0.2">
+        <v>20.808259027992921</v>
+      </c>
+      <c r="X33" s="12">
+        <f t="shared" si="1"/>
+        <v>73.968259027992914</v>
+      </c>
+    </row>
+    <row r="34" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B34" s="7"/>
       <c r="C34" s="5">
         <f>IFERROR(VLOOKUP(B34,'Location EPW.tsv'!$A$15:$L$230,12,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="D34" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="U34" s="10">
@@ -3865,17 +4379,21 @@
       </c>
       <c r="W34" s="12">
         <f t="shared" si="0"/>
-        <v>54.839999999999996</v>
-      </c>
-    </row>
-    <row r="35" spans="2:23" x14ac:dyDescent="0.2">
+        <v>20.78976641407921</v>
+      </c>
+      <c r="X34" s="12">
+        <f t="shared" si="1"/>
+        <v>75.629766414079214</v>
+      </c>
+    </row>
+    <row r="35" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B35" s="7"/>
       <c r="C35" s="5">
         <f>IFERROR(VLOOKUP(B35,'Location EPW.tsv'!$A$15:$L$230,12,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="D35" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="U35" s="10">
@@ -3887,17 +4405,21 @@
       </c>
       <c r="W35" s="12">
         <f t="shared" si="0"/>
-        <v>56.519999999999996</v>
-      </c>
-    </row>
-    <row r="36" spans="2:23" x14ac:dyDescent="0.2">
+        <v>20.772403120099156</v>
+      </c>
+      <c r="X35" s="12">
+        <f t="shared" si="1"/>
+        <v>77.292403120099152</v>
+      </c>
+    </row>
+    <row r="36" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B36" s="7"/>
       <c r="C36" s="5">
         <f>IFERROR(VLOOKUP(B36,'Location EPW.tsv'!$A$15:$L$230,12,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="D36" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="U36" s="10">
@@ -3909,17 +4431,21 @@
       </c>
       <c r="W36" s="12">
         <f t="shared" si="0"/>
-        <v>58.199999999999996</v>
-      </c>
-    </row>
-    <row r="37" spans="2:23" x14ac:dyDescent="0.2">
+        <v>20.756068762058653</v>
+      </c>
+      <c r="X36" s="12">
+        <f t="shared" si="1"/>
+        <v>78.956068762058649</v>
+      </c>
+    </row>
+    <row r="37" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B37" s="7"/>
       <c r="C37" s="5">
         <f>IFERROR(VLOOKUP(B37,'Location EPW.tsv'!$A$15:$L$230,12,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="D37" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="U37" s="10">
@@ -3931,17 +4457,21 @@
       </c>
       <c r="W37" s="12">
         <f t="shared" si="0"/>
-        <v>59.879999999999995</v>
-      </c>
-    </row>
-    <row r="38" spans="2:23" x14ac:dyDescent="0.2">
+        <v>20.740674510955738</v>
+      </c>
+      <c r="X37" s="12">
+        <f t="shared" si="1"/>
+        <v>80.620674510955737</v>
+      </c>
+    </row>
+    <row r="38" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B38" s="7"/>
       <c r="C38" s="5">
         <f>IFERROR(VLOOKUP(B38,'Location EPW.tsv'!$A$15:$L$230,12,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="D38" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="U38" s="10">
@@ -3953,17 +4483,21 @@
       </c>
       <c r="W38" s="12">
         <f t="shared" si="0"/>
-        <v>61.559999999999995</v>
-      </c>
-    </row>
-    <row r="39" spans="2:23" x14ac:dyDescent="0.2">
+        <v>20.726141476697745</v>
+      </c>
+      <c r="X38" s="12">
+        <f t="shared" si="1"/>
+        <v>82.286141476697736</v>
+      </c>
+    </row>
+    <row r="39" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B39" s="7"/>
       <c r="C39" s="5">
         <f>IFERROR(VLOOKUP(B39,'Location EPW.tsv'!$A$15:$L$230,12,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="D39" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="U39" s="10">
@@ -3975,17 +4509,21 @@
       </c>
       <c r="W39" s="12">
         <f t="shared" si="0"/>
-        <v>63.239999999999995</v>
-      </c>
-    </row>
-    <row r="40" spans="2:23" x14ac:dyDescent="0.2">
+        <v>20.712399355868758</v>
+      </c>
+      <c r="X39" s="12">
+        <f t="shared" si="1"/>
+        <v>83.952399355868764</v>
+      </c>
+    </row>
+    <row r="40" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B40" s="7"/>
       <c r="C40" s="5">
         <f>IFERROR(VLOOKUP(B40,'Location EPW.tsv'!$A$15:$L$230,12,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="D40" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="U40" s="10">
@@ -3997,17 +4535,21 @@
       </c>
       <c r="W40" s="12">
         <f t="shared" si="0"/>
-        <v>64.92</v>
-      </c>
-    </row>
-    <row r="41" spans="2:23" x14ac:dyDescent="0.2">
+        <v>20.69938529442144</v>
+      </c>
+      <c r="X40" s="12">
+        <f t="shared" si="1"/>
+        <v>85.619385294421448</v>
+      </c>
+    </row>
+    <row r="41" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B41" s="7"/>
       <c r="C41" s="5">
         <f>IFERROR(VLOOKUP(B41,'Location EPW.tsv'!$A$15:$L$230,12,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="D41" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="U41" s="10">
@@ -4019,17 +4561,21 @@
       </c>
       <c r="W41" s="12">
         <f t="shared" si="0"/>
-        <v>66.599999999999994</v>
-      </c>
-    </row>
-    <row r="42" spans="2:23" x14ac:dyDescent="0.2">
+        <v>20.68704292646817</v>
+      </c>
+      <c r="X41" s="12">
+        <f t="shared" si="1"/>
+        <v>87.287042926468175</v>
+      </c>
+    </row>
+    <row r="42" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B42" s="7"/>
       <c r="C42" s="5">
         <f>IFERROR(VLOOKUP(B42,'Location EPW.tsv'!$A$15:$L$230,12,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="D42" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="U42" s="10">
@@ -4041,17 +4587,21 @@
       </c>
       <c r="W42" s="12">
         <f t="shared" si="0"/>
-        <v>68.28</v>
-      </c>
-    </row>
-    <row r="43" spans="2:23" x14ac:dyDescent="0.2">
+        <v>20.675321558160356</v>
+      </c>
+      <c r="X42" s="12">
+        <f t="shared" si="1"/>
+        <v>88.955321558160335</v>
+      </c>
+    </row>
+    <row r="43" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B43" s="7"/>
       <c r="C43" s="5">
         <f>IFERROR(VLOOKUP(B43,'Location EPW.tsv'!$A$15:$L$230,12,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="D43" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="U43" s="10">
@@ -4063,17 +4613,21 @@
       </c>
       <c r="W43" s="12">
         <f t="shared" si="0"/>
-        <v>69.960000000000008</v>
-      </c>
-    </row>
-    <row r="44" spans="2:23" x14ac:dyDescent="0.2">
+        <v>20.664175471732673</v>
+      </c>
+      <c r="X43" s="12">
+        <f t="shared" si="1"/>
+        <v>90.62417547173267</v>
+      </c>
+    </row>
+    <row r="44" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B44" s="7"/>
       <c r="C44" s="5">
         <f>IFERROR(VLOOKUP(B44,'Location EPW.tsv'!$A$15:$L$230,12,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="D44" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="U44" s="10">
@@ -4085,17 +4639,21 @@
       </c>
       <c r="W44" s="12">
         <f t="shared" si="0"/>
-        <v>71.64</v>
-      </c>
-    </row>
-    <row r="45" spans="2:23" x14ac:dyDescent="0.2">
+        <v>20.653563329565003</v>
+      </c>
+      <c r="X44" s="12">
+        <f t="shared" si="1"/>
+        <v>92.293563329565004</v>
+      </c>
+    </row>
+    <row r="45" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B45" s="7"/>
       <c r="C45" s="5">
         <f>IFERROR(VLOOKUP(B45,'Location EPW.tsv'!$A$15:$L$230,12,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="D45" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="U45" s="10">
@@ -4107,17 +4665,21 @@
       </c>
       <c r="W45" s="12">
         <f t="shared" si="0"/>
-        <v>73.320000000000007</v>
-      </c>
-    </row>
-    <row r="46" spans="2:23" x14ac:dyDescent="0.2">
+        <v>20.643447661884711</v>
+      </c>
+      <c r="X45" s="12">
+        <f t="shared" si="1"/>
+        <v>93.9634476618847</v>
+      </c>
+    </row>
+    <row r="46" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B46" s="7"/>
       <c r="C46" s="5">
         <f>IFERROR(VLOOKUP(B46,'Location EPW.tsv'!$A$15:$L$230,12,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="D46" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="U46" s="10">
@@ -4129,17 +4691,21 @@
       </c>
       <c r="W46" s="12">
         <f t="shared" si="0"/>
-        <v>75</v>
-      </c>
-    </row>
-    <row r="47" spans="2:23" x14ac:dyDescent="0.2">
+        <v>20.63379442472694</v>
+      </c>
+      <c r="X46" s="12">
+        <f t="shared" si="1"/>
+        <v>95.633794424726943</v>
+      </c>
+    </row>
+    <row r="47" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B47" s="7"/>
       <c r="C47" s="5">
         <f>IFERROR(VLOOKUP(B47,'Location EPW.tsv'!$A$15:$L$230,12,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="D47" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="U47" s="10">
@@ -4151,17 +4717,21 @@
       </c>
       <c r="W47" s="12">
         <f t="shared" si="0"/>
-        <v>76.680000000000007</v>
-      </c>
-    </row>
-    <row r="48" spans="2:23" x14ac:dyDescent="0.2">
+        <v>20.624572617162816</v>
+      </c>
+      <c r="X47" s="12">
+        <f t="shared" si="1"/>
+        <v>97.304572617162819</v>
+      </c>
+    </row>
+    <row r="48" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B48" s="7"/>
       <c r="C48" s="5">
         <f>IFERROR(VLOOKUP(B48,'Location EPW.tsv'!$A$15:$L$230,12,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="D48" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="U48" s="10">
@@ -4173,17 +4743,21 @@
       </c>
       <c r="W48" s="12">
         <f t="shared" si="0"/>
-        <v>78.36</v>
-      </c>
-    </row>
-    <row r="49" spans="2:23" x14ac:dyDescent="0.2">
+        <v>20.615753948727178</v>
+      </c>
+      <c r="X48" s="12">
+        <f t="shared" si="1"/>
+        <v>98.975753948727188</v>
+      </c>
+    </row>
+    <row r="49" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B49" s="7"/>
       <c r="C49" s="5">
         <f>IFERROR(VLOOKUP(B49,'Location EPW.tsv'!$A$15:$L$230,12,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="D49" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="U49" s="10">
@@ -4195,17 +4769,21 @@
       </c>
       <c r="W49" s="12">
         <f t="shared" si="0"/>
-        <v>80.040000000000006</v>
-      </c>
-    </row>
-    <row r="50" spans="2:23" x14ac:dyDescent="0.2">
+        <v>20.607312549529432</v>
+      </c>
+      <c r="X49" s="12">
+        <f t="shared" si="1"/>
+        <v>100.64731254952943</v>
+      </c>
+    </row>
+    <row r="50" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B50" s="7"/>
       <c r="C50" s="5">
         <f>IFERROR(VLOOKUP(B50,'Location EPW.tsv'!$A$15:$L$230,12,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="D50" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="U50" s="10">
@@ -4217,17 +4795,21 @@
       </c>
       <c r="W50" s="12">
         <f t="shared" si="0"/>
-        <v>81.72</v>
-      </c>
-    </row>
-    <row r="51" spans="2:23" x14ac:dyDescent="0.2">
+        <v>20.599224716790225</v>
+      </c>
+      <c r="X50" s="12">
+        <f t="shared" si="1"/>
+        <v>102.31922471679022</v>
+      </c>
+    </row>
+    <row r="51" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B51" s="7"/>
       <c r="C51" s="5">
         <f>IFERROR(VLOOKUP(B51,'Location EPW.tsv'!$A$15:$L$230,12,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="D51" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="U51" s="10">
@@ -4239,17 +4821,21 @@
       </c>
       <c r="W51" s="12">
         <f t="shared" si="0"/>
-        <v>83.4</v>
-      </c>
-    </row>
-    <row r="52" spans="2:23" x14ac:dyDescent="0.2">
+        <v>20.591468692573653</v>
+      </c>
+      <c r="X51" s="12">
+        <f t="shared" si="1"/>
+        <v>103.99146869257365</v>
+      </c>
+    </row>
+    <row r="52" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B52" s="7"/>
       <c r="C52" s="5">
         <f>IFERROR(VLOOKUP(B52,'Location EPW.tsv'!$A$15:$L$230,12,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="D52" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="U52" s="10">
@@ -4261,17 +4847,21 @@
       </c>
       <c r="W52" s="12">
         <f t="shared" si="0"/>
-        <v>85.08</v>
-      </c>
-    </row>
-    <row r="53" spans="2:23" x14ac:dyDescent="0.2">
+        <v>20.584024468325588</v>
+      </c>
+      <c r="X52" s="12">
+        <f t="shared" si="1"/>
+        <v>105.66402446832558</v>
+      </c>
+    </row>
+    <row r="53" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B53" s="7"/>
       <c r="C53" s="5">
         <f>IFERROR(VLOOKUP(B53,'Location EPW.tsv'!$A$15:$L$230,12,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="D53" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="U53" s="10">
@@ -4283,17 +4873,21 @@
       </c>
       <c r="W53" s="12">
         <f t="shared" si="0"/>
-        <v>86.76</v>
-      </c>
-    </row>
-    <row r="54" spans="2:23" x14ac:dyDescent="0.2">
+        <v>20.576873612520796</v>
+      </c>
+      <c r="X53" s="12">
+        <f t="shared" si="1"/>
+        <v>107.33687361252079</v>
+      </c>
+    </row>
+    <row r="54" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B54" s="7"/>
       <c r="C54" s="5">
         <f>IFERROR(VLOOKUP(B54,'Location EPW.tsv'!$A$15:$L$230,12,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="D54" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="U54" s="10">
@@ -4305,116 +4899,120 @@
       </c>
       <c r="W54" s="12">
         <f t="shared" si="0"/>
-        <v>88.44</v>
-      </c>
-    </row>
-    <row r="55" spans="2:23" x14ac:dyDescent="0.2">
+        <v>20.569999118293001</v>
+      </c>
+      <c r="X54" s="12">
+        <f t="shared" si="1"/>
+        <v>109.009999118293</v>
+      </c>
+    </row>
+    <row r="55" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B55" s="7"/>
       <c r="C55" s="5">
         <f>IFERROR(VLOOKUP(B55,'Location EPW.tsv'!$A$15:$L$230,12,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="D55" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="2:23" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B56" s="7"/>
       <c r="C56" s="5">
         <f>IFERROR(VLOOKUP(B56,'Location EPW.tsv'!$A$15:$L$230,12,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="D56" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="2:23" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B57" s="7"/>
       <c r="C57" s="5">
         <f>IFERROR(VLOOKUP(B57,'Location EPW.tsv'!$A$15:$L$230,12,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="D57" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="2:23" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B58" s="7"/>
       <c r="C58" s="5">
         <f>IFERROR(VLOOKUP(B58,'Location EPW.tsv'!$A$15:$L$230,12,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="D58" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="2:23" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B59" s="7"/>
       <c r="C59" s="5">
         <f>IFERROR(VLOOKUP(B59,'Location EPW.tsv'!$A$15:$L$230,12,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="D59" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="2:23" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B60" s="7"/>
       <c r="C60" s="5">
         <f>IFERROR(VLOOKUP(B60,'Location EPW.tsv'!$A$15:$L$230,12,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="D60" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="2:23" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B61" s="7"/>
       <c r="C61" s="5">
         <f>IFERROR(VLOOKUP(B61,'Location EPW.tsv'!$A$15:$L$230,12,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="D61" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="2:23" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B62" s="7"/>
       <c r="C62" s="5">
         <f>IFERROR(VLOOKUP(B62,'Location EPW.tsv'!$A$15:$L$230,12,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="D62" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="2:23" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B63" s="7"/>
       <c r="C63" s="5">
         <f>IFERROR(VLOOKUP(B63,'Location EPW.tsv'!$A$15:$L$230,12,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="D63" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="2:23" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B64" s="7"/>
       <c r="C64" s="5">
         <f>IFERROR(VLOOKUP(B64,'Location EPW.tsv'!$A$15:$L$230,12,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="D64" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -4425,7 +5023,7 @@
         <v>0</v>
       </c>
       <c r="D65" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>